<commit_message>
[UPDATE] infoMessageBox msg updated
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7017" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7065" uniqueCount="1022">
   <si>
     <t>subject</t>
   </si>
@@ -3065,6 +3065,24 @@
   </si>
   <si>
     <t>230410_141657</t>
+  </si>
+  <si>
+    <t>230410_142150</t>
+  </si>
+  <si>
+    <t>230410_143622</t>
+  </si>
+  <si>
+    <t>230410_144300</t>
+  </si>
+  <si>
+    <t>230410_144515</t>
+  </si>
+  <si>
+    <t>230410_145010</t>
+  </si>
+  <si>
+    <t>230410_145033</t>
   </si>
 </sst>
 </file>
@@ -3770,7 +3788,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H870"/>
+  <dimension ref="A1:H876"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -26406,6 +26424,162 @@
         <v>996</v>
       </c>
     </row>
+    <row r="871" spans="1:8">
+      <c r="A871" t="s">
+        <v>10</v>
+      </c>
+      <c r="B871" t="s">
+        <v>998</v>
+      </c>
+      <c r="C871" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D871" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E871" t="s">
+        <v>986</v>
+      </c>
+      <c r="F871" t="s">
+        <v>990</v>
+      </c>
+      <c r="G871" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H871" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="872" spans="1:8">
+      <c r="A872" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B872" t="s">
+        <v>998</v>
+      </c>
+      <c r="C872" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D872" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E872" t="s">
+        <v>986</v>
+      </c>
+      <c r="F872" t="s">
+        <v>990</v>
+      </c>
+      <c r="G872" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H872" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="873" spans="1:8">
+      <c r="A873" t="s">
+        <v>10</v>
+      </c>
+      <c r="B873" t="s">
+        <v>998</v>
+      </c>
+      <c r="C873" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D873" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E873" t="s">
+        <v>986</v>
+      </c>
+      <c r="F873" t="s">
+        <v>990</v>
+      </c>
+      <c r="G873" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H873" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="874" spans="1:8">
+      <c r="A874" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B874" t="s">
+        <v>998</v>
+      </c>
+      <c r="C874" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D874" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E874" t="s">
+        <v>986</v>
+      </c>
+      <c r="F874" t="s">
+        <v>990</v>
+      </c>
+      <c r="G874" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H874" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="875" spans="1:8">
+      <c r="A875" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B875" t="s">
+        <v>998</v>
+      </c>
+      <c r="C875" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D875" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E875" t="s">
+        <v>986</v>
+      </c>
+      <c r="F875" t="s">
+        <v>990</v>
+      </c>
+      <c r="G875" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H875" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="876" spans="1:8">
+      <c r="A876" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B876" t="s">
+        <v>998</v>
+      </c>
+      <c r="C876" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D876" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E876" t="s">
+        <v>986</v>
+      </c>
+      <c r="F876" t="s">
+        <v>990</v>
+      </c>
+      <c r="G876" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H876" t="s">
+        <v>996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[FIX] fixed 'cancel' button of metadata.xlsx updating request
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george\Desktop\oqni\Recordings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E75133C-CF51-4887-9AA2-F4B929A673ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBDAFF6-B2B3-4971-A3A9-20B21B01D825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3416,7 +3416,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3727,8 +3727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H852"/>
   <sheetViews>
-    <sheetView topLeftCell="A837" workbookViewId="0">
-      <selection activeCell="C862" sqref="C862"/>
+    <sheetView topLeftCell="A826" workbookViewId="0">
+      <selection activeCell="A853" sqref="A853:XFD853"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[TEMP] draft to update
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7027" uniqueCount="1020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7083" uniqueCount="1027">
   <si>
     <t>subject</t>
   </si>
@@ -3077,6 +3077,27 @@
   </si>
   <si>
     <t>230416_170508</t>
+  </si>
+  <si>
+    <t>230416_171433</t>
+  </si>
+  <si>
+    <t>230416_171503</t>
+  </si>
+  <si>
+    <t>230416_171536</t>
+  </si>
+  <si>
+    <t>230416_171716</t>
+  </si>
+  <si>
+    <t>230416_171754</t>
+  </si>
+  <si>
+    <t>230416_173505</t>
+  </si>
+  <si>
+    <t>230416_174226</t>
   </si>
 </sst>
 </file>
@@ -3767,7 +3788,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H870"/>
+  <dimension ref="A1:H877"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -26393,6 +26414,188 @@
         <v>996</v>
       </c>
     </row>
+    <row r="871" spans="1:8">
+      <c r="A871" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B871" t="s">
+        <v>999</v>
+      </c>
+      <c r="C871" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D871" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E871" t="s">
+        <v>986</v>
+      </c>
+      <c r="F871" t="s">
+        <v>990</v>
+      </c>
+      <c r="G871" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H871" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="872" spans="1:8">
+      <c r="A872" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B872" t="s">
+        <v>999</v>
+      </c>
+      <c r="C872" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D872" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E872" t="s">
+        <v>986</v>
+      </c>
+      <c r="F872" t="s">
+        <v>990</v>
+      </c>
+      <c r="G872" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H872" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="873" spans="1:8">
+      <c r="A873" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B873" t="s">
+        <v>999</v>
+      </c>
+      <c r="C873" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D873" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E873" t="s">
+        <v>986</v>
+      </c>
+      <c r="F873" t="s">
+        <v>990</v>
+      </c>
+      <c r="G873" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H873" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="874" spans="1:8">
+      <c r="A874" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B874" t="s">
+        <v>999</v>
+      </c>
+      <c r="C874" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D874" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E874" t="s">
+        <v>986</v>
+      </c>
+      <c r="F874" t="s">
+        <v>990</v>
+      </c>
+      <c r="G874" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H874" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="875" spans="1:8">
+      <c r="A875" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B875" t="s">
+        <v>999</v>
+      </c>
+      <c r="C875" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D875" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E875" t="s">
+        <v>986</v>
+      </c>
+      <c r="F875" t="s">
+        <v>990</v>
+      </c>
+      <c r="G875" t="s">
+        <v>49</v>
+      </c>
+      <c r="H875" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="876" spans="1:8">
+      <c r="A876" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B876" t="s">
+        <v>999</v>
+      </c>
+      <c r="C876" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D876" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E876" t="s">
+        <v>986</v>
+      </c>
+      <c r="F876" t="s">
+        <v>990</v>
+      </c>
+      <c r="G876" t="s">
+        <v>49</v>
+      </c>
+      <c r="H876" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="877" spans="1:8">
+      <c r="A877" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B877" t="s">
+        <v>999</v>
+      </c>
+      <c r="C877" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D877" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E877" t="s">
+        <v>986</v>
+      </c>
+      <c r="F877" t="s">
+        <v>990</v>
+      </c>
+      <c r="G877" t="s">
+        <v>49</v>
+      </c>
+      <c r="H877" t="s">
+        <v>996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] autoscale finish (fix axis X on 10 sec.)
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7083" uniqueCount="1027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7121" uniqueCount="1034">
   <si>
     <t>subject</t>
   </si>
@@ -3098,6 +3098,27 @@
   </si>
   <si>
     <t>230416_174226</t>
+  </si>
+  <si>
+    <t>barev</t>
+  </si>
+  <si>
+    <t>BL-003_023_230420</t>
+  </si>
+  <si>
+    <t>230420_210634</t>
+  </si>
+  <si>
+    <t>230420_210658</t>
+  </si>
+  <si>
+    <t>230420_210804</t>
+  </si>
+  <si>
+    <t>230420_210907</t>
+  </si>
+  <si>
+    <t>230420_211015</t>
   </si>
 </sst>
 </file>
@@ -3645,7 +3666,7 @@
         <v>1011</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>1027</v>
       </c>
     </row>
   </sheetData>
@@ -3788,7 +3809,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H877"/>
+  <dimension ref="A1:H882"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -26596,6 +26617,136 @@
         <v>996</v>
       </c>
     </row>
+    <row r="878" spans="1:8">
+      <c r="A878" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B878" t="s">
+        <v>999</v>
+      </c>
+      <c r="C878" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D878" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E878" t="s">
+        <v>986</v>
+      </c>
+      <c r="F878" t="s">
+        <v>990</v>
+      </c>
+      <c r="G878" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H878" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="879" spans="1:8">
+      <c r="A879" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B879" t="s">
+        <v>999</v>
+      </c>
+      <c r="C879" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D879" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E879" t="s">
+        <v>986</v>
+      </c>
+      <c r="F879" t="s">
+        <v>990</v>
+      </c>
+      <c r="G879" t="s">
+        <v>49</v>
+      </c>
+      <c r="H879" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="880" spans="1:8">
+      <c r="A880" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B880" t="s">
+        <v>999</v>
+      </c>
+      <c r="C880" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D880" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E880" t="s">
+        <v>986</v>
+      </c>
+      <c r="F880" t="s">
+        <v>990</v>
+      </c>
+      <c r="G880" t="s">
+        <v>49</v>
+      </c>
+      <c r="H880" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="881" spans="1:8">
+      <c r="A881" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B881" t="s">
+        <v>999</v>
+      </c>
+      <c r="C881" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D881" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E881" t="s">
+        <v>986</v>
+      </c>
+      <c r="F881" t="s">
+        <v>990</v>
+      </c>
+      <c r="G881" t="s">
+        <v>49</v>
+      </c>
+      <c r="H881" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="882" spans="1:8">
+      <c r="A882" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B882" t="s">
+        <v>999</v>
+      </c>
+      <c r="C882" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D882" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E882" t="s">
+        <v>986</v>
+      </c>
+      <c r="F882" t="s">
+        <v>990</v>
+      </c>
+      <c r="G882" t="s">
+        <v>49</v>
+      </c>
+      <c r="H882" t="s">
+        <v>996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] starting work with new microcontroller ESP-32
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7125" uniqueCount="1035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7165" uniqueCount="1042">
   <si>
     <t>subject</t>
   </si>
@@ -3122,6 +3122,27 @@
   </si>
   <si>
     <t>024</t>
+  </si>
+  <si>
+    <t>BL-003_024_230526</t>
+  </si>
+  <si>
+    <t>230526_132306</t>
+  </si>
+  <si>
+    <t>230526_152003</t>
+  </si>
+  <si>
+    <t>BL-003_024_230527</t>
+  </si>
+  <si>
+    <t>230527_134750</t>
+  </si>
+  <si>
+    <t>230527_135055</t>
+  </si>
+  <si>
+    <t>230527_140127</t>
   </si>
 </sst>
 </file>
@@ -3820,7 +3841,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H882"/>
+  <dimension ref="A1:H887"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -26758,6 +26779,136 @@
         <v>996</v>
       </c>
     </row>
+    <row r="883" spans="1:8">
+      <c r="A883" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B883" t="s">
+        <v>999</v>
+      </c>
+      <c r="C883" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D883" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E883" t="s">
+        <v>986</v>
+      </c>
+      <c r="F883" t="s">
+        <v>990</v>
+      </c>
+      <c r="G883" t="s">
+        <v>49</v>
+      </c>
+      <c r="H883" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="884" spans="1:8">
+      <c r="A884" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B884" t="s">
+        <v>999</v>
+      </c>
+      <c r="C884" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D884" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E884" t="s">
+        <v>986</v>
+      </c>
+      <c r="F884" t="s">
+        <v>990</v>
+      </c>
+      <c r="G884" t="s">
+        <v>49</v>
+      </c>
+      <c r="H884" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="885" spans="1:8">
+      <c r="A885" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B885" t="s">
+        <v>999</v>
+      </c>
+      <c r="C885" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D885" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E885" t="s">
+        <v>986</v>
+      </c>
+      <c r="F885" t="s">
+        <v>990</v>
+      </c>
+      <c r="G885" t="s">
+        <v>49</v>
+      </c>
+      <c r="H885" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="886" spans="1:8">
+      <c r="A886" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B886" t="s">
+        <v>999</v>
+      </c>
+      <c r="C886" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D886" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E886" t="s">
+        <v>986</v>
+      </c>
+      <c r="F886" t="s">
+        <v>990</v>
+      </c>
+      <c r="G886" t="s">
+        <v>49</v>
+      </c>
+      <c r="H886" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="887" spans="1:8">
+      <c r="A887" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B887" t="s">
+        <v>999</v>
+      </c>
+      <c r="C887" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D887" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E887" t="s">
+        <v>986</v>
+      </c>
+      <c r="F887" t="s">
+        <v>990</v>
+      </c>
+      <c r="G887" t="s">
+        <v>49</v>
+      </c>
+      <c r="H887" t="s">
+        <v>996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] QByteArray changed to QVector<QByteArray>
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7165" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7171" uniqueCount="1043">
   <si>
     <t>subject</t>
   </si>
@@ -3143,6 +3143,9 @@
   </si>
   <si>
     <t>230527_140127</t>
+  </si>
+  <si>
+    <t>230527_165102</t>
   </si>
 </sst>
 </file>
@@ -3841,7 +3844,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H887"/>
+  <dimension ref="A1:H888"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -26909,6 +26912,32 @@
         <v>996</v>
       </c>
     </row>
+    <row r="888" spans="1:8">
+      <c r="A888" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B888" t="s">
+        <v>999</v>
+      </c>
+      <c r="C888" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D888" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E888" t="s">
+        <v>986</v>
+      </c>
+      <c r="F888" t="s">
+        <v>990</v>
+      </c>
+      <c r="G888" t="s">
+        <v>49</v>
+      </c>
+      <c r="H888" t="s">
+        <v>996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] saveToFile logic for ESP microcontroller
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7171" uniqueCount="1043">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7195" uniqueCount="1046">
   <si>
     <t>subject</t>
   </si>
@@ -3146,6 +3146,15 @@
   </si>
   <si>
     <t>230527_165102</t>
+  </si>
+  <si>
+    <t>230527_165906</t>
+  </si>
+  <si>
+    <t>230527_183302</t>
+  </si>
+  <si>
+    <t>230527_184903</t>
   </si>
 </sst>
 </file>
@@ -3844,7 +3853,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H888"/>
+  <dimension ref="A1:H891"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -26938,6 +26947,84 @@
         <v>996</v>
       </c>
     </row>
+    <row r="889" spans="1:8">
+      <c r="A889" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B889" t="s">
+        <v>999</v>
+      </c>
+      <c r="C889" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D889" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E889" t="s">
+        <v>986</v>
+      </c>
+      <c r="F889" t="s">
+        <v>990</v>
+      </c>
+      <c r="G889" t="s">
+        <v>49</v>
+      </c>
+      <c r="H889" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="890" spans="1:8">
+      <c r="A890" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B890" t="s">
+        <v>999</v>
+      </c>
+      <c r="C890" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D890" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E890" t="s">
+        <v>986</v>
+      </c>
+      <c r="F890" t="s">
+        <v>990</v>
+      </c>
+      <c r="G890" t="s">
+        <v>49</v>
+      </c>
+      <c r="H890" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="891" spans="1:8">
+      <c r="A891" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B891" t="s">
+        <v>999</v>
+      </c>
+      <c r="C891" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D891" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E891" t="s">
+        <v>986</v>
+      </c>
+      <c r="F891" t="s">
+        <v>990</v>
+      </c>
+      <c r="G891" t="s">
+        <v>993</v>
+      </c>
+      <c r="H891" t="s">
+        <v>996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[FIX] fixed label in the output file
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7195" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7227" uniqueCount="1050">
   <si>
     <t>subject</t>
   </si>
@@ -3155,6 +3155,18 @@
   </si>
   <si>
     <t>230527_184903</t>
+  </si>
+  <si>
+    <t>230527_211703</t>
+  </si>
+  <si>
+    <t>230527_214059</t>
+  </si>
+  <si>
+    <t>230527_221820</t>
+  </si>
+  <si>
+    <t>230527_221921</t>
   </si>
 </sst>
 </file>
@@ -3853,7 +3865,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H891"/>
+  <dimension ref="A1:H895"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -27025,6 +27037,110 @@
         <v>996</v>
       </c>
     </row>
+    <row r="892" spans="1:8">
+      <c r="A892" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B892" t="s">
+        <v>999</v>
+      </c>
+      <c r="C892" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D892" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E892" t="s">
+        <v>986</v>
+      </c>
+      <c r="F892" t="s">
+        <v>990</v>
+      </c>
+      <c r="G892" t="s">
+        <v>49</v>
+      </c>
+      <c r="H892" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="893" spans="1:8">
+      <c r="A893" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B893" t="s">
+        <v>999</v>
+      </c>
+      <c r="C893" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D893" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E893" t="s">
+        <v>986</v>
+      </c>
+      <c r="F893" t="s">
+        <v>990</v>
+      </c>
+      <c r="G893" t="s">
+        <v>49</v>
+      </c>
+      <c r="H893" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="894" spans="1:8">
+      <c r="A894" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B894" t="s">
+        <v>999</v>
+      </c>
+      <c r="C894" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D894" t="s">
+        <v>1048</v>
+      </c>
+      <c r="E894" t="s">
+        <v>986</v>
+      </c>
+      <c r="F894" t="s">
+        <v>990</v>
+      </c>
+      <c r="G894" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H894" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="895" spans="1:8">
+      <c r="A895" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B895" t="s">
+        <v>999</v>
+      </c>
+      <c r="C895" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D895" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E895" t="s">
+        <v>986</v>
+      </c>
+      <c r="F895" t="s">
+        <v>990</v>
+      </c>
+      <c r="G895" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H895" t="s">
+        <v>996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[FIX] fixed time (milliseconds) in the output file
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7227" uniqueCount="1050">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7269" uniqueCount="1056">
   <si>
     <t>subject</t>
   </si>
@@ -3167,6 +3167,24 @@
   </si>
   <si>
     <t>230527_221921</t>
+  </si>
+  <si>
+    <t>BL-003_024_230528</t>
+  </si>
+  <si>
+    <t>230528_003845</t>
+  </si>
+  <si>
+    <t>230528_004450</t>
+  </si>
+  <si>
+    <t>230528_004723</t>
+  </si>
+  <si>
+    <t>230528_011122</t>
+  </si>
+  <si>
+    <t>230528_012145</t>
   </si>
 </sst>
 </file>
@@ -3865,7 +3883,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H895"/>
+  <dimension ref="A1:H900"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -27141,6 +27159,136 @@
         <v>996</v>
       </c>
     </row>
+    <row r="896" spans="1:8">
+      <c r="A896" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B896" t="s">
+        <v>999</v>
+      </c>
+      <c r="C896" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D896" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E896" t="s">
+        <v>986</v>
+      </c>
+      <c r="F896" t="s">
+        <v>990</v>
+      </c>
+      <c r="G896" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H896" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="897" spans="1:8">
+      <c r="A897" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B897" t="s">
+        <v>999</v>
+      </c>
+      <c r="C897" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D897" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E897" t="s">
+        <v>986</v>
+      </c>
+      <c r="F897" t="s">
+        <v>990</v>
+      </c>
+      <c r="G897" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H897" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="898" spans="1:8">
+      <c r="A898" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B898" t="s">
+        <v>999</v>
+      </c>
+      <c r="C898" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D898" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E898" t="s">
+        <v>986</v>
+      </c>
+      <c r="F898" t="s">
+        <v>990</v>
+      </c>
+      <c r="G898" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H898" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="899" spans="1:8">
+      <c r="A899" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B899" t="s">
+        <v>999</v>
+      </c>
+      <c r="C899" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D899" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E899" t="s">
+        <v>986</v>
+      </c>
+      <c r="F899" t="s">
+        <v>990</v>
+      </c>
+      <c r="G899" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H899" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="900" spans="1:8">
+      <c r="A900" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B900" t="s">
+        <v>999</v>
+      </c>
+      <c r="C900" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D900" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E900" t="s">
+        <v>986</v>
+      </c>
+      <c r="F900" t="s">
+        <v>990</v>
+      </c>
+      <c r="G900" t="s">
+        <v>49</v>
+      </c>
+      <c r="H900" t="s">
+        <v>996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] oldCounter array changed from dynamic to static
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7269" uniqueCount="1056">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7275" uniqueCount="1057">
   <si>
     <t>subject</t>
   </si>
@@ -3185,6 +3185,9 @@
   </si>
   <si>
     <t>230528_012145</t>
+  </si>
+  <si>
+    <t>230528_014307</t>
   </si>
 </sst>
 </file>
@@ -3883,7 +3886,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H900"/>
+  <dimension ref="A1:H901"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -27289,6 +27292,32 @@
         <v>996</v>
       </c>
     </row>
+    <row r="901" spans="1:8">
+      <c r="A901" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B901" t="s">
+        <v>999</v>
+      </c>
+      <c r="C901" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D901" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E901" t="s">
+        <v>986</v>
+      </c>
+      <c r="F901" t="s">
+        <v>990</v>
+      </c>
+      <c r="G901" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H901" t="s">
+        <v>996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[ADD] initialization of first label in ctor
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7275" uniqueCount="1057">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7365" uniqueCount="1069">
   <si>
     <t>subject</t>
   </si>
@@ -3188,6 +3188,42 @@
   </si>
   <si>
     <t>230528_014307</t>
+  </si>
+  <si>
+    <t>230528_131721</t>
+  </si>
+  <si>
+    <t>230528_132300</t>
+  </si>
+  <si>
+    <t>230528_132914</t>
+  </si>
+  <si>
+    <t>Short#1_6s</t>
+  </si>
+  <si>
+    <t>230528_133103</t>
+  </si>
+  <si>
+    <t>230528_133250</t>
+  </si>
+  <si>
+    <t>230528_133501</t>
+  </si>
+  <si>
+    <t>230528_133716</t>
+  </si>
+  <si>
+    <t>230528_133812</t>
+  </si>
+  <si>
+    <t>230528_134242</t>
+  </si>
+  <si>
+    <t>230528_134616</t>
+  </si>
+  <si>
+    <t>230528_135602</t>
   </si>
 </sst>
 </file>
@@ -3886,7 +3922,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H901"/>
+  <dimension ref="A1:H912"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -27318,6 +27354,292 @@
         <v>996</v>
       </c>
     </row>
+    <row r="902" spans="1:8">
+      <c r="A902" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B902" t="s">
+        <v>999</v>
+      </c>
+      <c r="C902" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D902" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E902" t="s">
+        <v>986</v>
+      </c>
+      <c r="F902" t="s">
+        <v>990</v>
+      </c>
+      <c r="G902" t="s">
+        <v>49</v>
+      </c>
+      <c r="H902" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="903" spans="1:8">
+      <c r="A903" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B903" t="s">
+        <v>999</v>
+      </c>
+      <c r="C903" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D903" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E903" t="s">
+        <v>986</v>
+      </c>
+      <c r="F903" t="s">
+        <v>990</v>
+      </c>
+      <c r="G903" t="s">
+        <v>49</v>
+      </c>
+      <c r="H903" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="904" spans="1:8">
+      <c r="A904" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B904" t="s">
+        <v>999</v>
+      </c>
+      <c r="C904" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D904" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E904" t="s">
+        <v>986</v>
+      </c>
+      <c r="F904" t="s">
+        <v>990</v>
+      </c>
+      <c r="G904" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H904" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="905" spans="1:8">
+      <c r="A905" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B905" t="s">
+        <v>999</v>
+      </c>
+      <c r="C905" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D905" t="s">
+        <v>1061</v>
+      </c>
+      <c r="E905" t="s">
+        <v>986</v>
+      </c>
+      <c r="F905" t="s">
+        <v>990</v>
+      </c>
+      <c r="G905" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H905" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="906" spans="1:8">
+      <c r="A906" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B906" t="s">
+        <v>999</v>
+      </c>
+      <c r="C906" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D906" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E906" t="s">
+        <v>986</v>
+      </c>
+      <c r="F906" t="s">
+        <v>990</v>
+      </c>
+      <c r="G906" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H906" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="907" spans="1:8">
+      <c r="A907" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B907" t="s">
+        <v>999</v>
+      </c>
+      <c r="C907" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D907" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E907" t="s">
+        <v>986</v>
+      </c>
+      <c r="F907" t="s">
+        <v>990</v>
+      </c>
+      <c r="G907" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H907" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="908" spans="1:8">
+      <c r="A908" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B908" t="s">
+        <v>999</v>
+      </c>
+      <c r="C908" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D908" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E908" t="s">
+        <v>986</v>
+      </c>
+      <c r="F908" t="s">
+        <v>990</v>
+      </c>
+      <c r="G908" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H908" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="909" spans="1:8">
+      <c r="A909" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B909" t="s">
+        <v>999</v>
+      </c>
+      <c r="C909" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D909" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E909" t="s">
+        <v>986</v>
+      </c>
+      <c r="F909" t="s">
+        <v>990</v>
+      </c>
+      <c r="G909" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H909" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="910" spans="1:8">
+      <c r="A910" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B910" t="s">
+        <v>999</v>
+      </c>
+      <c r="C910" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D910" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E910" t="s">
+        <v>986</v>
+      </c>
+      <c r="F910" t="s">
+        <v>990</v>
+      </c>
+      <c r="G910" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H910" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="911" spans="1:8">
+      <c r="A911" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B911" t="s">
+        <v>999</v>
+      </c>
+      <c r="C911" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D911" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E911" t="s">
+        <v>986</v>
+      </c>
+      <c r="F911" t="s">
+        <v>990</v>
+      </c>
+      <c r="G911" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H911" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="912" spans="1:8">
+      <c r="A912" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B912" t="s">
+        <v>999</v>
+      </c>
+      <c r="C912" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D912" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E912" t="s">
+        <v>986</v>
+      </c>
+      <c r="F912" t="s">
+        <v>990</v>
+      </c>
+      <c r="G912" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H912" t="s">
+        <v>996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] updating dynamic chart design for best view
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7365" uniqueCount="1069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7379" uniqueCount="1073">
   <si>
     <t>subject</t>
   </si>
@@ -3224,6 +3224,18 @@
   </si>
   <si>
     <t>230528_135602</t>
+  </si>
+  <si>
+    <t>BL-003_024_230529</t>
+  </si>
+  <si>
+    <t>230529_193536</t>
+  </si>
+  <si>
+    <t>Exp#1_60s</t>
+  </si>
+  <si>
+    <t>230529_195124</t>
   </si>
 </sst>
 </file>
@@ -3922,7 +3934,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H912"/>
+  <dimension ref="A1:H914"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -27640,6 +27652,58 @@
         <v>996</v>
       </c>
     </row>
+    <row r="913" spans="1:8">
+      <c r="A913" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B913" t="s">
+        <v>999</v>
+      </c>
+      <c r="C913" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D913" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E913" t="s">
+        <v>986</v>
+      </c>
+      <c r="F913" t="s">
+        <v>990</v>
+      </c>
+      <c r="G913" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H913" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="914" spans="1:8">
+      <c r="A914" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B914" t="s">
+        <v>999</v>
+      </c>
+      <c r="C914" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D914" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E914" t="s">
+        <v>986</v>
+      </c>
+      <c r="F914" t="s">
+        <v>990</v>
+      </c>
+      <c r="G914" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H914" t="s">
+        <v>996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] using header <algorithm>
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7379" uniqueCount="1073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7381" uniqueCount="1073">
   <si>
     <t>subject</t>
   </si>

</xml_diff>

<commit_message>
[ADD] send label to the MC, read it and write to the file
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7381" uniqueCount="1073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7443" uniqueCount="1082">
   <si>
     <t>subject</t>
   </si>
@@ -3236,6 +3236,33 @@
   </si>
   <si>
     <t>230529_195124</t>
+  </si>
+  <si>
+    <t>230529_203532</t>
+  </si>
+  <si>
+    <t>230529_205305</t>
+  </si>
+  <si>
+    <t>230529_214509</t>
+  </si>
+  <si>
+    <t>230529_222553</t>
+  </si>
+  <si>
+    <t>230529_222816</t>
+  </si>
+  <si>
+    <t>Exp#5_14s</t>
+  </si>
+  <si>
+    <t>230529_223403</t>
+  </si>
+  <si>
+    <t>230529_223559</t>
+  </si>
+  <si>
+    <t>230529_224049</t>
   </si>
 </sst>
 </file>
@@ -3934,7 +3961,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H914"/>
+  <dimension ref="A1:H922"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -27704,6 +27731,214 @@
         <v>996</v>
       </c>
     </row>
+    <row r="915" spans="1:8">
+      <c r="A915" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B915" t="s">
+        <v>999</v>
+      </c>
+      <c r="C915" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D915" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E915" t="s">
+        <v>986</v>
+      </c>
+      <c r="F915" t="s">
+        <v>990</v>
+      </c>
+      <c r="G915" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H915" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="916" spans="1:8">
+      <c r="A916" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B916" t="s">
+        <v>999</v>
+      </c>
+      <c r="C916" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D916" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E916" t="s">
+        <v>986</v>
+      </c>
+      <c r="F916" t="s">
+        <v>990</v>
+      </c>
+      <c r="G916" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H916" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="917" spans="1:8">
+      <c r="A917" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B917" t="s">
+        <v>999</v>
+      </c>
+      <c r="C917" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D917" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E917" t="s">
+        <v>986</v>
+      </c>
+      <c r="F917" t="s">
+        <v>990</v>
+      </c>
+      <c r="G917" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H917" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="918" spans="1:8">
+      <c r="A918" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B918" t="s">
+        <v>999</v>
+      </c>
+      <c r="C918" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D918" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E918" t="s">
+        <v>986</v>
+      </c>
+      <c r="F918" t="s">
+        <v>990</v>
+      </c>
+      <c r="G918" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H918" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="919" spans="1:8">
+      <c r="A919" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B919" t="s">
+        <v>999</v>
+      </c>
+      <c r="C919" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D919" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E919" t="s">
+        <v>986</v>
+      </c>
+      <c r="F919" t="s">
+        <v>990</v>
+      </c>
+      <c r="G919" t="s">
+        <v>1078</v>
+      </c>
+      <c r="H919" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="920" spans="1:8">
+      <c r="A920" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B920" t="s">
+        <v>999</v>
+      </c>
+      <c r="C920" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D920" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E920" t="s">
+        <v>986</v>
+      </c>
+      <c r="F920" t="s">
+        <v>990</v>
+      </c>
+      <c r="G920" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H920" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="921" spans="1:8">
+      <c r="A921" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B921" t="s">
+        <v>999</v>
+      </c>
+      <c r="C921" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D921" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E921" t="s">
+        <v>986</v>
+      </c>
+      <c r="F921" t="s">
+        <v>990</v>
+      </c>
+      <c r="G921" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H921" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="922" spans="1:8">
+      <c r="A922" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B922" t="s">
+        <v>999</v>
+      </c>
+      <c r="C922" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D922" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E922" t="s">
+        <v>986</v>
+      </c>
+      <c r="F922" t="s">
+        <v>990</v>
+      </c>
+      <c r="G922" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H922" t="s">
+        <v>996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] disconnect(this->_threadDisplayTimer, &ThreadDisplayTimer::currentLabel, this, nullptr);
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7443" uniqueCount="1082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7445" uniqueCount="1082">
   <si>
     <t>subject</t>
   </si>

</xml_diff>

<commit_message>
[ADD] reading Time Counter from MC and writing in the .csv file
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7445" uniqueCount="1082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7603" uniqueCount="1103">
   <si>
     <t>subject</t>
   </si>
@@ -3263,6 +3263,69 @@
   </si>
   <si>
     <t>230529_224049</t>
+  </si>
+  <si>
+    <t>BL-003_024_230530</t>
+  </si>
+  <si>
+    <t>230530_113523</t>
+  </si>
+  <si>
+    <t>230530_113845</t>
+  </si>
+  <si>
+    <t>230530_115123</t>
+  </si>
+  <si>
+    <t>230530_120934</t>
+  </si>
+  <si>
+    <t>230530_122720</t>
+  </si>
+  <si>
+    <t>230530_124547</t>
+  </si>
+  <si>
+    <t>230530_125056</t>
+  </si>
+  <si>
+    <t>230530_125439</t>
+  </si>
+  <si>
+    <t>230530_130747</t>
+  </si>
+  <si>
+    <t>230530_131220</t>
+  </si>
+  <si>
+    <t>230530_132329</t>
+  </si>
+  <si>
+    <t>230530_132527</t>
+  </si>
+  <si>
+    <t>230530_132832</t>
+  </si>
+  <si>
+    <t>230530_133313</t>
+  </si>
+  <si>
+    <t>230530_133611</t>
+  </si>
+  <si>
+    <t>230530_134658</t>
+  </si>
+  <si>
+    <t>230530_135617</t>
+  </si>
+  <si>
+    <t>230530_135815</t>
+  </si>
+  <si>
+    <t>230530_135940</t>
+  </si>
+  <si>
+    <t>230530_140005</t>
   </si>
 </sst>
 </file>
@@ -3961,7 +4024,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H922"/>
+  <dimension ref="A1:H942"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -27939,6 +28002,526 @@
         <v>996</v>
       </c>
     </row>
+    <row r="923" spans="1:8">
+      <c r="A923" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B923" t="s">
+        <v>999</v>
+      </c>
+      <c r="C923" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D923" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E923" t="s">
+        <v>986</v>
+      </c>
+      <c r="F923" t="s">
+        <v>990</v>
+      </c>
+      <c r="G923" t="s">
+        <v>1078</v>
+      </c>
+      <c r="H923" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="924" spans="1:8">
+      <c r="A924" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B924" t="s">
+        <v>999</v>
+      </c>
+      <c r="C924" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D924" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E924" t="s">
+        <v>986</v>
+      </c>
+      <c r="F924" t="s">
+        <v>990</v>
+      </c>
+      <c r="G924" t="s">
+        <v>1078</v>
+      </c>
+      <c r="H924" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="925" spans="1:8">
+      <c r="A925" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B925" t="s">
+        <v>999</v>
+      </c>
+      <c r="C925" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D925" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E925" t="s">
+        <v>986</v>
+      </c>
+      <c r="F925" t="s">
+        <v>990</v>
+      </c>
+      <c r="G925" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H925" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="926" spans="1:8">
+      <c r="A926" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B926" t="s">
+        <v>999</v>
+      </c>
+      <c r="C926" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D926" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E926" t="s">
+        <v>986</v>
+      </c>
+      <c r="F926" t="s">
+        <v>990</v>
+      </c>
+      <c r="G926" t="s">
+        <v>1078</v>
+      </c>
+      <c r="H926" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="927" spans="1:8">
+      <c r="A927" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B927" t="s">
+        <v>999</v>
+      </c>
+      <c r="C927" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D927" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E927" t="s">
+        <v>986</v>
+      </c>
+      <c r="F927" t="s">
+        <v>990</v>
+      </c>
+      <c r="G927" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H927" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="928" spans="1:8">
+      <c r="A928" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B928" t="s">
+        <v>999</v>
+      </c>
+      <c r="C928" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D928" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E928" t="s">
+        <v>986</v>
+      </c>
+      <c r="F928" t="s">
+        <v>990</v>
+      </c>
+      <c r="G928" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H928" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="929" spans="1:8">
+      <c r="A929" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B929" t="s">
+        <v>999</v>
+      </c>
+      <c r="C929" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D929" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E929" t="s">
+        <v>986</v>
+      </c>
+      <c r="F929" t="s">
+        <v>990</v>
+      </c>
+      <c r="G929" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H929" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="930" spans="1:8">
+      <c r="A930" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B930" t="s">
+        <v>999</v>
+      </c>
+      <c r="C930" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D930" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E930" t="s">
+        <v>986</v>
+      </c>
+      <c r="F930" t="s">
+        <v>990</v>
+      </c>
+      <c r="G930" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H930" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="931" spans="1:8">
+      <c r="A931" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B931" t="s">
+        <v>999</v>
+      </c>
+      <c r="C931" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D931" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E931" t="s">
+        <v>986</v>
+      </c>
+      <c r="F931" t="s">
+        <v>990</v>
+      </c>
+      <c r="G931" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H931" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="932" spans="1:8">
+      <c r="A932" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B932" t="s">
+        <v>999</v>
+      </c>
+      <c r="C932" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D932" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E932" t="s">
+        <v>986</v>
+      </c>
+      <c r="F932" t="s">
+        <v>990</v>
+      </c>
+      <c r="G932" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H932" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="933" spans="1:8">
+      <c r="A933" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B933" t="s">
+        <v>999</v>
+      </c>
+      <c r="C933" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D933" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E933" t="s">
+        <v>986</v>
+      </c>
+      <c r="F933" t="s">
+        <v>990</v>
+      </c>
+      <c r="G933" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H933" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="934" spans="1:8">
+      <c r="A934" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B934" t="s">
+        <v>999</v>
+      </c>
+      <c r="C934" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D934" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E934" t="s">
+        <v>986</v>
+      </c>
+      <c r="F934" t="s">
+        <v>990</v>
+      </c>
+      <c r="G934" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H934" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="935" spans="1:8">
+      <c r="A935" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B935" t="s">
+        <v>999</v>
+      </c>
+      <c r="C935" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D935" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E935" t="s">
+        <v>986</v>
+      </c>
+      <c r="F935" t="s">
+        <v>990</v>
+      </c>
+      <c r="G935" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H935" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="936" spans="1:8">
+      <c r="A936" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B936" t="s">
+        <v>999</v>
+      </c>
+      <c r="C936" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D936" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E936" t="s">
+        <v>986</v>
+      </c>
+      <c r="F936" t="s">
+        <v>990</v>
+      </c>
+      <c r="G936" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H936" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="937" spans="1:8">
+      <c r="A937" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B937" t="s">
+        <v>999</v>
+      </c>
+      <c r="C937" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D937" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E937" t="s">
+        <v>986</v>
+      </c>
+      <c r="F937" t="s">
+        <v>990</v>
+      </c>
+      <c r="G937" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H937" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="938" spans="1:8">
+      <c r="A938" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B938" t="s">
+        <v>999</v>
+      </c>
+      <c r="C938" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D938" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E938" t="s">
+        <v>986</v>
+      </c>
+      <c r="F938" t="s">
+        <v>990</v>
+      </c>
+      <c r="G938" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H938" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="939" spans="1:8">
+      <c r="A939" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B939" t="s">
+        <v>999</v>
+      </c>
+      <c r="C939" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D939" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E939" t="s">
+        <v>986</v>
+      </c>
+      <c r="F939" t="s">
+        <v>990</v>
+      </c>
+      <c r="G939" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H939" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="940" spans="1:8">
+      <c r="A940" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B940" t="s">
+        <v>999</v>
+      </c>
+      <c r="C940" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D940" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E940" t="s">
+        <v>986</v>
+      </c>
+      <c r="F940" t="s">
+        <v>990</v>
+      </c>
+      <c r="G940" t="s">
+        <v>1078</v>
+      </c>
+      <c r="H940" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="941" spans="1:8">
+      <c r="A941" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B941" t="s">
+        <v>999</v>
+      </c>
+      <c r="C941" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D941" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E941" t="s">
+        <v>986</v>
+      </c>
+      <c r="F941" t="s">
+        <v>990</v>
+      </c>
+      <c r="G941" t="s">
+        <v>1078</v>
+      </c>
+      <c r="H941" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="942" spans="1:8">
+      <c r="A942" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B942" t="s">
+        <v>999</v>
+      </c>
+      <c r="C942" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D942" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E942" t="s">
+        <v>986</v>
+      </c>
+      <c r="F942" t="s">
+        <v>990</v>
+      </c>
+      <c r="G942" t="s">
+        <v>1078</v>
+      </c>
+      <c r="H942" t="s">
+        <v>996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] Infrared and green swapped on windowchart
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7691" uniqueCount="1119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7701" uniqueCount="1120">
   <si>
     <t>subject</t>
   </si>
@@ -3375,6 +3375,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>230531_144757</t>
   </si>
 </sst>
 </file>
@@ -4107,7 +4110,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J952"/>
+  <dimension ref="A1:J953"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -28889,6 +28892,38 @@
         <v>1105</v>
       </c>
     </row>
+    <row r="953" spans="1:10">
+      <c r="A953" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B953" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C953" s="4" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D953" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E953" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F953" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G953" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H953" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I953" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J953" s="4" t="s">
+        <v>1105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] save light intensity and distance at the start
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7701" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7711" uniqueCount="1122">
   <si>
     <t>subject</t>
   </si>
@@ -3378,6 +3378,12 @@
   </si>
   <si>
     <t>230531_144757</t>
+  </si>
+  <si>
+    <t>230531_170530</t>
+  </si>
+  <si>
+    <t>35, 35, 35</t>
   </si>
 </sst>
 </file>
@@ -4110,7 +4116,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J953"/>
+  <dimension ref="A1:J954"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -28924,6 +28930,38 @@
         <v>1105</v>
       </c>
     </row>
+    <row r="954" spans="1:10">
+      <c r="A954" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B954" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C954" s="4" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D954" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E954" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F954" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G954" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="H954" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I954" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J954" s="4" t="s">
+        <v>1105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28953,7 +28991,7 @@
         <v>1118</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1105</v>
+        <v>1121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UPDATE] Separate function for filling series and updating axes for OPT sensors.
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7711" uniqueCount="1122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7730" uniqueCount="1124">
   <si>
     <t>subject</t>
   </si>
@@ -3384,6 +3384,12 @@
   </si>
   <si>
     <t>35, 35, 35</t>
+  </si>
+  <si>
+    <t>230531_174737</t>
+  </si>
+  <si>
+    <t>230531_175522</t>
   </si>
 </sst>
 </file>
@@ -4116,7 +4122,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J954"/>
+  <dimension ref="A1:J956"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -28962,6 +28968,70 @@
         <v>1105</v>
       </c>
     </row>
+    <row r="955" spans="1:10">
+      <c r="A955" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B955" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C955" s="4" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D955" s="4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="E955" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F955" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G955" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H955" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I955" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J955" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="956" spans="1:10">
+      <c r="A956" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B956" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C956" s="4" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D956" s="4" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E956" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F956" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G956" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="H956" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I956" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J956" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] defining _sliderHorizontal style
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7730" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7731" uniqueCount="1124">
   <si>
     <t>subject</t>
   </si>

</xml_diff>

<commit_message>
[ADD] added checkBoxes on dynamic chart window for selecting sensor
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7731" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7760" uniqueCount="1127">
   <si>
     <t>subject</t>
   </si>
@@ -3390,6 +3390,15 @@
   </si>
   <si>
     <t>230531_175522</t>
+  </si>
+  <si>
+    <t>230531_204437</t>
+  </si>
+  <si>
+    <t>230531_205106</t>
+  </si>
+  <si>
+    <t>230531_205404</t>
   </si>
 </sst>
 </file>
@@ -4122,7 +4131,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J956"/>
+  <dimension ref="A1:J959"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -29032,6 +29041,102 @@
         <v>1121</v>
       </c>
     </row>
+    <row r="957" spans="1:10">
+      <c r="A957" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B957" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C957" s="4" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D957" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="E957" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F957" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G957" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H957" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I957" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J957" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="958" spans="1:10">
+      <c r="A958" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B958" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C958" s="4" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D958" s="4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E958" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F958" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G958" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H958" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I958" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J958" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="959" spans="1:10">
+      <c r="A959" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B959" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C959" s="4" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D959" s="4" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E959" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F959" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G959" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H959" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I959" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J959" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[ADD] created an array _chartView_IMU for IMU sensors and inserted into the dynamic chart window
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7760" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7810" uniqueCount="1134">
   <si>
     <t>subject</t>
   </si>
@@ -3399,6 +3399,27 @@
   </si>
   <si>
     <t>230531_205404</t>
+  </si>
+  <si>
+    <t>BL-003_025_230601</t>
+  </si>
+  <si>
+    <t>230601_002851</t>
+  </si>
+  <si>
+    <t>Exp#4_113s</t>
+  </si>
+  <si>
+    <t>230601_013013</t>
+  </si>
+  <si>
+    <t>230601_021131</t>
+  </si>
+  <si>
+    <t>230601_140111</t>
+  </si>
+  <si>
+    <t>230601_171210</t>
   </si>
 </sst>
 </file>
@@ -4131,7 +4152,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J959"/>
+  <dimension ref="A1:J964"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -28699,7 +28720,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="945" spans="1:10">
+    <row r="945" spans="1:8">
       <c r="A945" s="4" t="s">
         <v>1107</v>
       </c>
@@ -28725,7 +28746,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="946" spans="1:10">
+    <row r="946" spans="1:8">
       <c r="A946" s="4" t="s">
         <v>1107</v>
       </c>
@@ -28751,7 +28772,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="947" spans="1:10">
+    <row r="947" spans="1:8">
       <c r="A947" s="4" t="s">
         <v>1107</v>
       </c>
@@ -28777,7 +28798,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="948" spans="1:10">
+    <row r="948" spans="1:8">
       <c r="A948" s="4" t="s">
         <v>1107</v>
       </c>
@@ -28803,7 +28824,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="949" spans="1:10">
+    <row r="949" spans="1:8">
       <c r="A949" s="4" t="s">
         <v>1107</v>
       </c>
@@ -28829,7 +28850,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="950" spans="1:10">
+    <row r="950" spans="1:8">
       <c r="A950" s="4" t="s">
         <v>1107</v>
       </c>
@@ -28855,7 +28876,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="951" spans="1:10">
+    <row r="951" spans="1:8">
       <c r="A951" s="4" t="s">
         <v>1107</v>
       </c>
@@ -28881,7 +28902,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="952" spans="1:10">
+    <row r="952" spans="1:8">
       <c r="A952" s="4" t="s">
         <v>1107</v>
       </c>
@@ -28913,7 +28934,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="953" spans="1:10">
+    <row r="953" spans="1:8">
       <c r="A953" s="4" t="s">
         <v>1107</v>
       </c>
@@ -28945,7 +28966,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="954" spans="1:10">
+    <row r="954" spans="1:8">
       <c r="A954" s="4" t="s">
         <v>1107</v>
       </c>
@@ -28977,7 +28998,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="955" spans="1:10">
+    <row r="955" spans="1:8">
       <c r="A955" s="4" t="s">
         <v>1107</v>
       </c>
@@ -29009,7 +29030,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="956" spans="1:10">
+    <row r="956" spans="1:8">
       <c r="A956" s="4" t="s">
         <v>1107</v>
       </c>
@@ -29041,7 +29062,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="957" spans="1:10">
+    <row r="957" spans="1:8">
       <c r="A957" s="4" t="s">
         <v>1107</v>
       </c>
@@ -29073,7 +29094,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="958" spans="1:10">
+    <row r="958" spans="1:8">
       <c r="A958" s="4" t="s">
         <v>1107</v>
       </c>
@@ -29105,7 +29126,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="959" spans="1:10">
+    <row r="959" spans="1:8">
       <c r="A959" s="4" t="s">
         <v>1107</v>
       </c>
@@ -29134,6 +29155,166 @@
         <v>1118</v>
       </c>
       <c r="J959" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="960" spans="1:8">
+      <c r="A960" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B960" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C960" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D960" s="4" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E960" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F960" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G960" s="4" t="s">
+        <v>1129</v>
+      </c>
+      <c r="H960" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I960" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J960" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="961" spans="1:10">
+      <c r="A961" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B961" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C961" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D961" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="E961" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F961" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G961" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H961" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I961" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J961" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="962" spans="1:10">
+      <c r="A962" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B962" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C962" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D962" s="4" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E962" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F962" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G962" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H962" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I962" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J962" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="963" spans="1:10">
+      <c r="A963" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B963" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C963" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D963" s="4" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E963" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F963" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G963" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H963" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I963" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J963" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="964" spans="1:10">
+      <c r="A964" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B964" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C964" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D964" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E964" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F964" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G964" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H964" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I964" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J964" s="4" t="s">
         <v>1121</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[ADD]  set the stretch factor for the rows on dynamic chart
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7810" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7820" uniqueCount="1136">
   <si>
     <t>subject</t>
   </si>
@@ -3420,6 +3420,12 @@
   </si>
   <si>
     <t>230601_171210</t>
+  </si>
+  <si>
+    <t>BL-003_025_230602</t>
+  </si>
+  <si>
+    <t>230602_015346</t>
   </si>
 </sst>
 </file>
@@ -4152,7 +4158,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J964"/>
+  <dimension ref="A1:J965"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -29318,6 +29324,38 @@
         <v>1121</v>
       </c>
     </row>
+    <row r="965" spans="1:10">
+      <c r="A965" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B965" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C965" s="4" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D965" s="4" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E965" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F965" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G965" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H965" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I965" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J965" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] renaming _series variables to _series_OPT
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7820" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7841" uniqueCount="1138">
   <si>
     <t>subject</t>
   </si>
@@ -3426,6 +3426,12 @@
   </si>
   <si>
     <t>230602_015346</t>
+  </si>
+  <si>
+    <t>230602_130856</t>
+  </si>
+  <si>
+    <t>230602_131037</t>
   </si>
 </sst>
 </file>
@@ -4158,7 +4164,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J965"/>
+  <dimension ref="A1:J967"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -29356,6 +29362,70 @@
         <v>1121</v>
       </c>
     </row>
+    <row r="966" spans="1:10">
+      <c r="A966" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B966" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C966" s="4" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D966" s="4" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E966" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F966" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G966" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H966" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I966" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J966" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="967" spans="1:10">
+      <c r="A967" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B967" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C967" s="4" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D967" s="4" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E967" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F967" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G967" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H967" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I967" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J967" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[FIX] bug fixed (int to short)
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7841" uniqueCount="1138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7850" uniqueCount="1139">
   <si>
     <t>subject</t>
   </si>
@@ -3432,6 +3432,9 @@
   </si>
   <si>
     <t>230602_131037</t>
+  </si>
+  <si>
+    <t>230602_234654</t>
   </si>
 </sst>
 </file>
@@ -4164,7 +4167,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J967"/>
+  <dimension ref="A1:J968"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -29426,6 +29429,38 @@
         <v>1121</v>
       </c>
     </row>
+    <row r="968" spans="1:10">
+      <c r="A968" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B968" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C968" s="4" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D968" s="4" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E968" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F968" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G968" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H968" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I968" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J968" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[FIX] fixed short min/max
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7850" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7851" uniqueCount="1139">
   <si>
     <t>subject</t>
   </si>

</xml_diff>

<commit_message>
[UPDAE] set chart duration 5 sec.
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7851" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7860" uniqueCount="1141">
   <si>
     <t>subject</t>
   </si>
@@ -3435,6 +3435,12 @@
   </si>
   <si>
     <t>230602_234654</t>
+  </si>
+  <si>
+    <t>BL-003_025_230603</t>
+  </si>
+  <si>
+    <t>230603_232600</t>
   </si>
 </sst>
 </file>
@@ -4167,7 +4173,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J968"/>
+  <dimension ref="A1:J969"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -29461,6 +29467,38 @@
         <v>1121</v>
       </c>
     </row>
+    <row r="969" spans="1:10">
+      <c r="A969" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B969" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C969" s="4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D969" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E969" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F969" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G969" s="4" t="s">
+        <v>1129</v>
+      </c>
+      <c r="H969" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I969" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J969" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[ADD] multiset for OPT sensors
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7860" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7861" uniqueCount="1140">
   <si>
     <t>subject</t>
   </si>
@@ -3434,13 +3434,10 @@
     <t>230602_131037</t>
   </si>
   <si>
-    <t>230602_234654</t>
-  </si>
-  <si>
-    <t>BL-003_025_230603</t>
-  </si>
-  <si>
-    <t>230603_232600</t>
+    <t>230602_172216</t>
+  </si>
+  <si>
+    <t>230602_200551</t>
   </si>
 </sst>
 </file>
@@ -29475,11 +29472,11 @@
         <v>999</v>
       </c>
       <c r="C969" s="4" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D969" s="4" t="s">
         <v>1139</v>
       </c>
-      <c r="D969" s="4" t="s">
-        <v>1140</v>
-      </c>
       <c r="E969" s="4" t="s">
         <v>986</v>
       </c>
@@ -29487,7 +29484,7 @@
         <v>990</v>
       </c>
       <c r="G969" s="4" t="s">
-        <v>1129</v>
+        <v>1070</v>
       </c>
       <c r="H969" s="4" t="s">
         <v>996</v>

</xml_diff>

<commit_message>
[UPDATE] set chart duration range [2, 6] seconds
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7861" uniqueCount="1140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7870" uniqueCount="1142">
   <si>
     <t>subject</t>
   </si>
@@ -3438,6 +3438,12 @@
   </si>
   <si>
     <t>230602_200551</t>
+  </si>
+  <si>
+    <t>BL-003_025_230604</t>
+  </si>
+  <si>
+    <t>230604_232745</t>
   </si>
 </sst>
 </file>
@@ -4170,7 +4176,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J969"/>
+  <dimension ref="A1:J970"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -29496,6 +29502,38 @@
         <v>1121</v>
       </c>
     </row>
+    <row r="970" spans="1:10">
+      <c r="A970" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B970" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C970" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D970" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E970" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F970" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G970" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H970" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I970" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J970" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] combining functions ..._autoscale_... and ..._NoAutoscale_...
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7870" uniqueCount="1142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7881" uniqueCount="1143">
   <si>
     <t>subject</t>
   </si>
@@ -3444,6 +3444,9 @@
   </si>
   <si>
     <t>230604_232745</t>
+  </si>
+  <si>
+    <t>230604_235243</t>
   </si>
 </sst>
 </file>
@@ -4176,7 +4179,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J970"/>
+  <dimension ref="A1:J971"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -29534,6 +29537,38 @@
         <v>1121</v>
       </c>
     </row>
+    <row r="971" spans="1:10">
+      <c r="A971" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B971" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C971" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D971" s="4" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E971" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F971" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G971" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H971" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I971" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J971" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] reformating Comport ctor initialization list
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7881" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7931" uniqueCount="1149">
   <si>
     <t>subject</t>
   </si>
@@ -3447,6 +3447,24 @@
   </si>
   <si>
     <t>230604_235243</t>
+  </si>
+  <si>
+    <t>BL-003_025_230605</t>
+  </si>
+  <si>
+    <t>230605_205438</t>
+  </si>
+  <si>
+    <t>230605_211055</t>
+  </si>
+  <si>
+    <t>230605_211207</t>
+  </si>
+  <si>
+    <t>230605_211602</t>
+  </si>
+  <si>
+    <t>230605_212045</t>
   </si>
 </sst>
 </file>
@@ -4179,7 +4197,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J971"/>
+  <dimension ref="A1:J976"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -29569,6 +29587,166 @@
         <v>1121</v>
       </c>
     </row>
+    <row r="972" spans="1:10">
+      <c r="A972" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B972" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C972" s="4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D972" s="4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E972" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F972" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G972" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H972" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I972" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J972" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="973" spans="1:10">
+      <c r="A973" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B973" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C973" s="4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D973" s="4" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E973" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F973" s="4" t="s">
+        <v>991</v>
+      </c>
+      <c r="G973" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H973" s="4" t="s">
+        <v>997</v>
+      </c>
+      <c r="I973" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J973" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="974" spans="1:10">
+      <c r="A974" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B974" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C974" s="4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D974" s="4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E974" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F974" s="4" t="s">
+        <v>991</v>
+      </c>
+      <c r="G974" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H974" s="4" t="s">
+        <v>997</v>
+      </c>
+      <c r="I974" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J974" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="975" spans="1:10">
+      <c r="A975" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B975" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C975" s="4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D975" s="4" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E975" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F975" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G975" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H975" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I975" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J975" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="976" spans="1:10">
+      <c r="A976" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B976" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C976" s="4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D976" s="4" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E976" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F976" s="4" t="s">
+        <v>991</v>
+      </c>
+      <c r="G976" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H976" s="4" t="s">
+        <v>997</v>
+      </c>
+      <c r="I976" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J976" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] if duration is set to 0, enable test mode 23:59:59
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7931" uniqueCount="1149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7941" uniqueCount="1151">
   <si>
     <t>subject</t>
   </si>
@@ -3465,6 +3465,12 @@
   </si>
   <si>
     <t>230605_212045</t>
+  </si>
+  <si>
+    <t>BL-003_025_230606</t>
+  </si>
+  <si>
+    <t>230606_004650</t>
   </si>
 </sst>
 </file>
@@ -4197,7 +4203,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J976"/>
+  <dimension ref="A1:J977"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -29747,6 +29753,38 @@
         <v>1121</v>
       </c>
     </row>
+    <row r="977" spans="1:10">
+      <c r="A977" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B977" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C977" s="4" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D977" s="4" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E977" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F977" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G977" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="H977" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I977" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J977" s="4" t="s">
+        <v>1121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29773,10 +29811,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>1118</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UPDATE] using <algorithm> in _windowchart.hpp
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7950" uniqueCount="1152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7951" uniqueCount="1152">
   <si>
     <t>subject</t>
   </si>

</xml_diff>

<commit_message>
[ADD] added _snapshotButton functionality
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7960" uniqueCount="1154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7969" uniqueCount="1156">
   <si>
     <t>subject</t>
   </si>
@@ -3480,6 +3480,12 @@
   </si>
   <si>
     <t>230607_234556</t>
+  </si>
+  <si>
+    <t>BL-003_025_230612</t>
+  </si>
+  <si>
+    <t>230612_221935</t>
   </si>
 </sst>
 </file>
@@ -4212,7 +4218,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J979"/>
+  <dimension ref="A1:J980"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -29858,6 +29864,38 @@
         <v>1118</v>
       </c>
     </row>
+    <row r="980" spans="1:10">
+      <c r="A980" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B980" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C980" s="4" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D980" s="4" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E980" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F980" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G980" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H980" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I980" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J980" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[ADD] added icons to QMessageBox-es
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7969" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8050" uniqueCount="1165">
   <si>
     <t>subject</t>
   </si>
@@ -3486,6 +3486,33 @@
   </si>
   <si>
     <t>230612_221935</t>
+  </si>
+  <si>
+    <t>BL-003_025_230613</t>
+  </si>
+  <si>
+    <t>230613_133946</t>
+  </si>
+  <si>
+    <t>230613_135455</t>
+  </si>
+  <si>
+    <t>230613_135708</t>
+  </si>
+  <si>
+    <t>230613_135819</t>
+  </si>
+  <si>
+    <t>230613_140252</t>
+  </si>
+  <si>
+    <t>230613_140439</t>
+  </si>
+  <si>
+    <t>230613_143824</t>
+  </si>
+  <si>
+    <t>230613_145439</t>
   </si>
 </sst>
 </file>
@@ -4218,7 +4245,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J980"/>
+  <dimension ref="A1:J988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -29896,6 +29923,262 @@
         <v>1118</v>
       </c>
     </row>
+    <row r="981" spans="1:10">
+      <c r="A981" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B981" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C981" s="4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D981" s="4" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E981" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F981" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G981" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H981" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I981" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J981" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="982" spans="1:10">
+      <c r="A982" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B982" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C982" s="4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D982" s="4" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E982" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F982" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G982" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H982" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I982" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J982" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="983" spans="1:10">
+      <c r="A983" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B983" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C983" s="4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D983" s="4" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E983" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F983" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G983" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H983" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I983" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J983" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="984" spans="1:10">
+      <c r="A984" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B984" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C984" s="4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D984" s="4" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E984" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F984" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G984" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H984" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I984" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J984" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="985" spans="1:10">
+      <c r="A985" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B985" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C985" s="4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D985" s="4" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E985" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F985" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G985" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H985" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I985" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J985" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="986" spans="1:10">
+      <c r="A986" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B986" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C986" s="4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D986" s="4" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E986" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F986" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G986" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H986" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I986" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J986" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="987" spans="1:10">
+      <c r="A987" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B987" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C987" s="4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D987" s="4" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E987" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F987" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G987" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H987" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I987" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J987" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="988" spans="1:10">
+      <c r="A988" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B988" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C988" s="4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D988" s="4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E988" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F988" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G988" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H988" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I988" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J988" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[ADD] added warning QMessageBox for wrong ID
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8050" uniqueCount="1165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8070" uniqueCount="1167">
   <si>
     <t>subject</t>
   </si>
@@ -3513,6 +3513,12 @@
   </si>
   <si>
     <t>230613_145439</t>
+  </si>
+  <si>
+    <t>230613_164609</t>
+  </si>
+  <si>
+    <t>230613_202639</t>
   </si>
 </sst>
 </file>
@@ -4245,7 +4251,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J988"/>
+  <dimension ref="A1:J990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -30179,6 +30185,70 @@
         <v>1118</v>
       </c>
     </row>
+    <row r="989" spans="1:10">
+      <c r="A989" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B989" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C989" s="4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D989" s="4" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E989" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F989" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G989" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H989" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I989" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J989" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="990" spans="1:10">
+      <c r="A990" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B990" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C990" s="4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D990" s="4" t="s">
+        <v>1166</v>
+      </c>
+      <c r="E990" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F990" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G990" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H990" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I990" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J990" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] code style optimization
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8070" uniqueCount="1167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8109" uniqueCount="1173">
   <si>
     <t>subject</t>
   </si>
@@ -3519,6 +3519,24 @@
   </si>
   <si>
     <t>230613_202639</t>
+  </si>
+  <si>
+    <t>BL-003_024_230614</t>
+  </si>
+  <si>
+    <t>230614_142821</t>
+  </si>
+  <si>
+    <t>BL-003_025_230614</t>
+  </si>
+  <si>
+    <t>230614_145845</t>
+  </si>
+  <si>
+    <t>230614_145951</t>
+  </si>
+  <si>
+    <t>230614_161241</t>
   </si>
 </sst>
 </file>
@@ -4251,7 +4269,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J990"/>
+  <dimension ref="A1:J994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -30249,6 +30267,134 @@
         <v>1118</v>
       </c>
     </row>
+    <row r="991" spans="1:10">
+      <c r="A991" s="4" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B991" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C991" s="4" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D991" s="4" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E991" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F991" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G991" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H991" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I991" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J991" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="992" spans="1:10">
+      <c r="A992" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B992" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C992" s="4" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D992" s="4" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E992" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F992" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G992" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H992" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I992" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J992" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="993" spans="1:10">
+      <c r="A993" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B993" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C993" s="4" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D993" s="4" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E993" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F993" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G993" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H993" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I993" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J993" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="994" spans="1:10">
+      <c r="A994" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B994" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C994" s="4" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D994" s="4" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E994" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F994" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G994" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H994" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I994" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J994" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[UPDATE] slider horizontal resized
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8109" uniqueCount="1173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8110" uniqueCount="1173">
   <si>
     <t>subject</t>
   </si>

</xml_diff>

<commit_message>
[ADD] replacing the first row with the second row for OPT sensors, as requested by Naira
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8110" uniqueCount="1173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8279" uniqueCount="1192">
   <si>
     <t>subject</t>
   </si>
@@ -3537,6 +3537,63 @@
   </si>
   <si>
     <t>230614_161241</t>
+  </si>
+  <si>
+    <t>BL-003_025_230619</t>
+  </si>
+  <si>
+    <t>230619_235230</t>
+  </si>
+  <si>
+    <t>230619_235558</t>
+  </si>
+  <si>
+    <t>BL-003_025_230620</t>
+  </si>
+  <si>
+    <t>230620_002256</t>
+  </si>
+  <si>
+    <t>230620_002719</t>
+  </si>
+  <si>
+    <t>230620_003239</t>
+  </si>
+  <si>
+    <t>230620_003430</t>
+  </si>
+  <si>
+    <t>230620_003443</t>
+  </si>
+  <si>
+    <t>230620_003713</t>
+  </si>
+  <si>
+    <t>230620_003756</t>
+  </si>
+  <si>
+    <t>230620_004343</t>
+  </si>
+  <si>
+    <t>230620_005035</t>
+  </si>
+  <si>
+    <t>230620_005851</t>
+  </si>
+  <si>
+    <t>230620_010150</t>
+  </si>
+  <si>
+    <t>230620_011017</t>
+  </si>
+  <si>
+    <t>230620_012151</t>
+  </si>
+  <si>
+    <t>230620_012558</t>
+  </si>
+  <si>
+    <t>230620_012711</t>
   </si>
 </sst>
 </file>
@@ -4269,7 +4326,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J994"/>
+  <dimension ref="A1:J1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -30395,6 +30452,550 @@
         <v>1118</v>
       </c>
     </row>
+    <row r="995" spans="1:10">
+      <c r="A995" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B995" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C995" s="4" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D995" s="4" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E995" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F995" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G995" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H995" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I995" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J995" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="996" spans="1:10">
+      <c r="A996" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B996" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C996" s="4" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D996" s="4" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E996" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F996" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G996" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H996" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I996" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J996" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="997" spans="1:10">
+      <c r="A997" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B997" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C997" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D997" s="4" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E997" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F997" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G997" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H997" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I997" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J997" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="998" spans="1:10">
+      <c r="A998" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B998" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C998" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D998" s="4" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E998" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F998" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G998" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H998" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I998" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J998" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="999" spans="1:10">
+      <c r="A999" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B999" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C999" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D999" s="4" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E999" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F999" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G999" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H999" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I999" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J999" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:10">
+      <c r="A1000" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1000" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C1000" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D1000" s="4" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E1000" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F1000" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G1000" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H1000" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I1000" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J1000" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:10">
+      <c r="A1001" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1001" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C1001" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D1001" s="4" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E1001" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F1001" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G1001" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H1001" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I1001" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J1001" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:10">
+      <c r="A1002" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1002" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C1002" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D1002" s="4" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E1002" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F1002" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G1002" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H1002" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I1002" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J1002" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:10">
+      <c r="A1003" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1003" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C1003" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D1003" s="4" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E1003" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F1003" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G1003" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H1003" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I1003" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J1003" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:10">
+      <c r="A1004" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1004" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C1004" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D1004" s="4" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E1004" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F1004" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G1004" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H1004" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I1004" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J1004" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:10">
+      <c r="A1005" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1005" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C1005" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D1005" s="4" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E1005" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F1005" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G1005" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H1005" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I1005" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J1005" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:10">
+      <c r="A1006" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1006" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C1006" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D1006" s="4" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E1006" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F1006" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G1006" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H1006" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I1006" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J1006" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:10">
+      <c r="A1007" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1007" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C1007" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D1007" s="4" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E1007" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F1007" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G1007" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H1007" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I1007" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J1007" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:10">
+      <c r="A1008" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1008" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C1008" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D1008" s="4" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E1008" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F1008" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G1008" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H1008" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I1008" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J1008" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:10">
+      <c r="A1009" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1009" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C1009" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D1009" s="4" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E1009" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F1009" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G1009" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H1009" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I1009" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J1009" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:10">
+      <c r="A1010" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1010" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C1010" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D1010" s="4" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E1010" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F1010" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G1010" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H1010" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I1010" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J1010" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:10">
+      <c r="A1011" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1011" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C1011" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D1011" s="4" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E1011" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="F1011" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="G1011" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H1011" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="I1011" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J1011" s="4" t="s">
+        <v>1118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[FIX] processing gif fixed
</commit_message>
<xml_diff>
--- a/Recordings/metadata.xlsx
+++ b/Recordings/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8279" uniqueCount="1192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8280" uniqueCount="1192">
   <si>
     <t>subject</t>
   </si>

</xml_diff>